<commit_message>
Demonstrament 001 | Pilers
</commit_message>
<xml_diff>
--- a/designment/projects/001/docubase/docubase.xlsx
+++ b/designment/projects/001/docubase/docubase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="VINE" sheetId="1" state="visible" r:id="rId3"/>
@@ -16,6 +16,7 @@
     <sheet name="VERS_0_Docubase_Pages" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="VERS_4_Docubase_Pages" sheetId="7" state="hidden" r:id="rId9"/>
     <sheet name="VIEW_0_Docubase_Page_Views" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="VELI_0_Docubase_Page_Styles" sheetId="9" state="hidden" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="AREA" vbProcedure="false">VINE!$A$1:$CI$46</definedName>
@@ -87,6 +88,13 @@
     <definedName function="false" hidden="false" localSheetId="7" name="MOD_0" vbProcedure="false">VIEW_0_Docubase_Page_Views!$A$1:$AV$56</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="MOD_0_COM" vbProcedure="false">VIEW_0_Docubase_Page_Views!$A$5:$AV$56</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="MOD_0_SUP" vbProcedure="false">VIEW_0_Docubase_Page_Views!$A$1:$AV$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="AREA" vbProcedure="false">VELI_0_Docubase_Page_Styles!$A$1:$X$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="LMN_0" vbProcedure="false">VELI_0_Docubase_Page_Styles!$F$1:$M$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="LMN_0_SUBSET" vbProcedure="false">VELI_0_Docubase_Page_Styles!$D$1:$D$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="LMN_0_SUPSET" vbProcedure="false">VELI_0_Docubase_Page_Styles!$C$1:$C$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="MOD_0" vbProcedure="false">VELI_0_Docubase_Page_Styles!$A$1:$X$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="MOD_0_COM" vbProcedure="false">VELI_0_Docubase_Page_Styles!$A$5:$X$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="MOD_0_SUP" vbProcedure="false">VELI_0_Docubase_Page_Styles!$A$1:$X$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -98,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3130" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3156" uniqueCount="461">
   <si>
     <t xml:space="preserve">fs</t>
   </si>
@@ -4557,7 +4565,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L35" activeCellId="0" sqref="L35"/>
+      <selection pane="bottomRight" activeCell="I49" activeCellId="0" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18381,11 +18389,11 @@
   <dimension ref="A1:AA116"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="XEP40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="XEP1" activeCellId="0" sqref="XEP1"/>
-      <selection pane="bottomLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
-      <selection pane="bottomRight" activeCell="XFD49" activeCellId="0" sqref="XFD49"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="M35" activeCellId="0" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
@@ -22439,7 +22447,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -24113,12 +24121,12 @@
   </sheetPr>
   <dimension ref="A1:AK83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="S36" activeCellId="0" sqref="S36"/>
+      <selection pane="bottomRight" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -28298,12 +28306,12 @@
   </sheetPr>
   <dimension ref="A1:AW57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="13" ySplit="4" topLeftCell="N5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J34" activeCellId="0" sqref="J34"/>
+      <selection pane="bottomRight" activeCell="AF21" activeCellId="0" sqref="AF21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31988,4 +31996,478 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FF01579B"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AA25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="A11" activeCellId="0" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="3" width="2.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="65" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="6" style="1" width="4.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="7.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="2" width="3.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="5.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="42.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="5.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="21" style="1" width="3.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="4.91"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="26" min="26" style="1" width="50.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="35.99"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="165" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="165"/>
+      <c r="C1" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
+      <c r="R1" s="167" t="s">
+        <v>105</v>
+      </c>
+      <c r="S1" s="167"/>
+      <c r="T1" s="167"/>
+      <c r="U1" s="167"/>
+      <c r="V1" s="167"/>
+      <c r="W1" s="167"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="72" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA1" s="72" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="165" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="166" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="168" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="168" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="166" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="166"/>
+      <c r="G2" s="166"/>
+      <c r="H2" s="166"/>
+      <c r="I2" s="166"/>
+      <c r="J2" s="166"/>
+      <c r="K2" s="166"/>
+      <c r="L2" s="166"/>
+      <c r="M2" s="166"/>
+      <c r="N2" s="166"/>
+      <c r="O2" s="166"/>
+      <c r="P2" s="166"/>
+      <c r="Q2" s="166"/>
+      <c r="R2" s="165" t="s">
+        <v>112</v>
+      </c>
+      <c r="S2" s="165"/>
+      <c r="T2" s="165"/>
+      <c r="U2" s="165"/>
+      <c r="V2" s="165"/>
+      <c r="W2" s="165"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="72"/>
+      <c r="AA2" s="72"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="165"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="166" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="165" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="165"/>
+      <c r="H3" s="165"/>
+      <c r="I3" s="165"/>
+      <c r="J3" s="165"/>
+      <c r="K3" s="165"/>
+      <c r="L3" s="165"/>
+      <c r="M3" s="165"/>
+      <c r="N3" s="166" t="s">
+        <v>115</v>
+      </c>
+      <c r="O3" s="166" t="s">
+        <v>116</v>
+      </c>
+      <c r="P3" s="166"/>
+      <c r="Q3" s="166" t="s">
+        <v>117</v>
+      </c>
+      <c r="R3" s="168" t="s">
+        <v>113</v>
+      </c>
+      <c r="S3" s="165" t="s">
+        <v>114</v>
+      </c>
+      <c r="T3" s="165" t="s">
+        <v>115</v>
+      </c>
+      <c r="U3" s="165" t="s">
+        <v>116</v>
+      </c>
+      <c r="V3" s="165"/>
+      <c r="W3" s="165" t="s">
+        <v>117</v>
+      </c>
+      <c r="X3" s="70"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="72"/>
+      <c r="AA3" s="72"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="165"/>
+      <c r="B4" s="166"/>
+      <c r="C4" s="168"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="165"/>
+      <c r="G4" s="165"/>
+      <c r="H4" s="165"/>
+      <c r="I4" s="165"/>
+      <c r="J4" s="165"/>
+      <c r="K4" s="165"/>
+      <c r="L4" s="165"/>
+      <c r="M4" s="165"/>
+      <c r="N4" s="166"/>
+      <c r="O4" s="166" t="s">
+        <v>118</v>
+      </c>
+      <c r="P4" s="166" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q4" s="166"/>
+      <c r="R4" s="168"/>
+      <c r="S4" s="165"/>
+      <c r="T4" s="165"/>
+      <c r="U4" s="165" t="s">
+        <v>118</v>
+      </c>
+      <c r="V4" s="165" t="s">
+        <v>119</v>
+      </c>
+      <c r="W4" s="165"/>
+      <c r="X4" s="70"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="75"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
+      <c r="R5" s="77"/>
+      <c r="S5" s="77"/>
+      <c r="T5" s="169"/>
+      <c r="U5" s="77"/>
+      <c r="V5" s="77"/>
+      <c r="W5" s="77"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="78"/>
+      <c r="Z5" s="93"/>
+      <c r="AA5" s="93"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="80"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="170"/>
+      <c r="F6" s="171"/>
+      <c r="G6" s="171"/>
+      <c r="H6" s="171"/>
+      <c r="I6" s="171"/>
+      <c r="J6" s="171"/>
+      <c r="K6" s="171"/>
+      <c r="L6" s="171"/>
+      <c r="M6" s="171"/>
+      <c r="N6" s="172"/>
+      <c r="O6" s="173"/>
+      <c r="P6" s="174"/>
+      <c r="Q6" s="175"/>
+      <c r="R6" s="170"/>
+      <c r="S6" s="176"/>
+      <c r="T6" s="172"/>
+      <c r="U6" s="173"/>
+      <c r="V6" s="174"/>
+      <c r="W6" s="172"/>
+      <c r="X6" s="70"/>
+      <c r="Y6" s="59"/>
+      <c r="Z6" s="93"/>
+      <c r="AA6" s="93"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="70"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="70"/>
+      <c r="Q7" s="70"/>
+      <c r="R7" s="70"/>
+      <c r="S7" s="70"/>
+      <c r="T7" s="285"/>
+      <c r="U7" s="70"/>
+      <c r="V7" s="70"/>
+      <c r="W7" s="70"/>
+      <c r="X7" s="70"/>
+      <c r="Y7" s="59"/>
+      <c r="Z7" s="93"/>
+      <c r="AA7" s="93"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="59"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="123" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="123" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="123" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="123" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" s="123" t="n">
+        <v>4</v>
+      </c>
+      <c r="K8" s="123" t="n">
+        <v>5</v>
+      </c>
+      <c r="L8" s="123" t="n">
+        <v>6</v>
+      </c>
+      <c r="M8" s="123" t="n">
+        <v>7</v>
+      </c>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="59"/>
+      <c r="Q8" s="59"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="62"/>
+      <c r="U8" s="59"/>
+      <c r="V8" s="59"/>
+      <c r="W8" s="59"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="59"/>
+      <c r="Z8" s="93"/>
+      <c r="AA8" s="93"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:Q1"/>
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="Z1:Z4"/>
+    <mergeCell ref="AA1:AA4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:Q2"/>
+    <mergeCell ref="R2:W2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:W4"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Demonstrament 001 | Pages - Index
</commit_message>
<xml_diff>
--- a/designment/projects/001/docubase/docubase.xlsx
+++ b/designment/projects/001/docubase/docubase.xlsx
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3778" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3790" uniqueCount="535">
   <si>
     <t xml:space="preserve">fs</t>
   </si>
@@ -15159,11 +15159,11 @@
   <dimension ref="A1:AA185"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E157" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
-      <selection pane="bottomRight" activeCell="L24" activeCellId="0" sqref="L24"/>
+      <selection pane="bottomLeft" activeCell="A157" activeCellId="0" sqref="A157"/>
+      <selection pane="bottomRight" activeCell="D179" activeCellId="0" sqref="D179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -22356,7 +22356,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="R90" activeCellId="0" sqref="R90"/>
+      <selection pane="bottomRight" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -32655,11 +32655,11 @@
   <dimension ref="A1:AW65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="13" ySplit="4" topLeftCell="N5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="13" ySplit="4" topLeftCell="N38" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="C64" activeCellId="0" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33125,8 +33125,12 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="396"/>
       <c r="B7" s="396"/>
-      <c r="C7" s="397"/>
-      <c r="D7" s="398"/>
+      <c r="C7" s="397" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="398" t="s">
+        <v>458</v>
+      </c>
       <c r="E7" s="399"/>
       <c r="F7" s="399"/>
       <c r="G7" s="399"/>
@@ -33180,8 +33184,12 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="396"/>
       <c r="B8" s="396"/>
-      <c r="C8" s="397"/>
-      <c r="D8" s="398"/>
+      <c r="C8" s="397" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="398" t="s">
+        <v>458</v>
+      </c>
       <c r="E8" s="399"/>
       <c r="F8" s="399"/>
       <c r="G8" s="399"/>
@@ -33418,8 +33426,12 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="396"/>
       <c r="B12" s="396"/>
-      <c r="C12" s="397"/>
-      <c r="D12" s="398"/>
+      <c r="C12" s="397" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="398" t="s">
+        <v>458</v>
+      </c>
       <c r="E12" s="399"/>
       <c r="F12" s="399"/>
       <c r="G12" s="399"/>
@@ -33473,8 +33485,12 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="396"/>
       <c r="B13" s="396"/>
-      <c r="C13" s="397"/>
-      <c r="D13" s="398"/>
+      <c r="C13" s="397" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="398" t="s">
+        <v>458</v>
+      </c>
       <c r="E13" s="399"/>
       <c r="F13" s="399"/>
       <c r="G13" s="399"/>
@@ -33530,8 +33546,12 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="396"/>
       <c r="B14" s="396"/>
-      <c r="C14" s="397"/>
-      <c r="D14" s="398"/>
+      <c r="C14" s="397" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="398" t="s">
+        <v>458</v>
+      </c>
       <c r="E14" s="399"/>
       <c r="F14" s="399"/>
       <c r="G14" s="399"/>
@@ -33589,8 +33609,12 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="396"/>
       <c r="B15" s="396"/>
-      <c r="C15" s="397"/>
-      <c r="D15" s="398"/>
+      <c r="C15" s="397" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="398" t="s">
+        <v>458</v>
+      </c>
       <c r="E15" s="399"/>
       <c r="F15" s="399"/>
       <c r="G15" s="399"/>

</xml_diff>

<commit_message>
DFC | Generator Templates
</commit_message>
<xml_diff>
--- a/designment/projects/001/docubase/docubase.xlsx
+++ b/designment/projects/001/docubase/docubase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="VINE" sheetId="1" state="visible" r:id="rId3"/>
@@ -58,15 +58,15 @@
     <definedName function="false" hidden="false" localSheetId="4" name="MOD_0" vbProcedure="false">VERS_0_Docubase_Application!$A$1:$X$35</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="MOD_0_COM" vbProcedure="false">VERS_0_Docubase_Application!$A$5:$X$35</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="MOD_0_SUP" vbProcedure="false">VERS_0_Docubase_Application!$A$1:$X$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="AREA" vbProcedure="false">VERS_0_Docubase_Pages!$A$1:$X$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="LMN_0" vbProcedure="false">VERS_0_Docubase_Pages!$F$1:$M$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="LMN_0_SUBSET" vbProcedure="false">VERS_0_Docubase_Pages!$D$1:$D$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="LMN_0_SUPSET" vbProcedure="false">VERS_0_Docubase_Pages!$C$1:$C$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="AREA" vbProcedure="false">VERS_0_Docubase_Pages!$A$1:$X$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="LMN_0" vbProcedure="false">VERS_0_Docubase_Pages!$F$1:$M$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="LMN_0_SUBSET" vbProcedure="false">VERS_0_Docubase_Pages!$D$1:$D$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="LMN_0_SUPSET" vbProcedure="false">VERS_0_Docubase_Pages!$C$1:$C$45</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="LMN_1" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="LMN_1_SUBSET" vbProcedure="false">VERS_0_Docubase_Pages!$D$1:$D$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="LMN_1_SUPSET" vbProcedure="false">VERS_0_Docubase_Pages!$C$1:$C$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="MOD_0" vbProcedure="false">VERS_0_Docubase_Pages!$A$1:$X$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="MOD_0_COM" vbProcedure="false">VERS_0_Docubase_Pages!$A$5:$X$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="LMN_1_SUBSET" vbProcedure="false">VERS_0_Docubase_Pages!$D$1:$D$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="LMN_1_SUPSET" vbProcedure="false">VERS_0_Docubase_Pages!$C$1:$C$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="MOD_0" vbProcedure="false">VERS_0_Docubase_Pages!$A$1:$X$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="MOD_0_COM" vbProcedure="false">VERS_0_Docubase_Pages!$A$5:$X$45</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="MOD_0_SUP" vbProcedure="false">VERS_0_Docubase_Pages!$A$1:$X$4</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="AREA" vbProcedure="false">VIEW_0_Docubase_Page_Templates!$A$1:$AV$55</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="LMN_0" vbProcedure="false">VIEW_0_Docubase_Page_Templates!$W$1:$AE$55</definedName>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3873" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3884" uniqueCount="539">
   <si>
     <t xml:space="preserve">fs</t>
   </si>
@@ -982,25 +982,7 @@
     <t xml:space="preserve">'develop/templates/html/html5'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="FreeMono"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="FreeMono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">index'</t>
-    </r>
+    <t xml:space="preserve">'index'</t>
   </si>
   <si>
     <t xml:space="preserve">outputName</t>
@@ -1411,6 +1393,9 @@
     <t xml:space="preserve">Pages | Index - JSON</t>
   </si>
   <si>
+    <t xml:space="preserve">"app"</t>
+  </si>
+  <si>
     <t xml:space="preserve">"meta"</t>
   </si>
   <si>
@@ -1705,7 +1690,7 @@
     <t xml:space="preserve">Docubase | Pages - Index</t>
   </si>
   <si>
-    <t xml:space="preserve">div</t>
+    <t xml:space="preserve">app</t>
   </si>
   <si>
     <t xml:space="preserve">"Hello All Dogs"</t>
@@ -1751,7 +1736,7 @@
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1888,12 +1873,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="FreeMono"/>
-      <family val="3"/>
     </font>
     <font>
       <b val="true"/>
@@ -2040,7 +2019,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFC530F"/>
-        <bgColor rgb="FFFA4808"/>
+        <bgColor rgb="FFF84807"/>
       </patternFill>
     </fill>
     <fill>
@@ -2117,7 +2096,7 @@
     </fill>
     <fill>
       <patternFill patternType="darkGray">
-        <fgColor rgb="FFFEE1A3"/>
+        <fgColor rgb="FFFEE1A6"/>
         <bgColor rgb="FFFFD63B"/>
       </patternFill>
     </fill>
@@ -2201,7 +2180,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF85B739"/>
+        <fgColor rgb="FF85B839"/>
         <bgColor rgb="FF99CC61"/>
       </patternFill>
     </fill>
@@ -2255,7 +2234,7 @@
     </fill>
     <fill>
       <patternFill patternType="darkGray">
-        <fgColor rgb="FFFEE1A3"/>
+        <fgColor rgb="FFFEE1A6"/>
         <bgColor rgb="FFF3E5F5"/>
       </patternFill>
     </fill>
@@ -2279,13 +2258,13 @@
     </fill>
     <fill>
       <patternFill patternType="darkGray">
-        <fgColor rgb="FF85B739"/>
+        <fgColor rgb="FF85B839"/>
         <bgColor rgb="FF99CC61"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFA4808"/>
+        <fgColor rgb="FFF84807"/>
         <bgColor rgb="FFFC530F"/>
       </patternFill>
     </fill>
@@ -2420,14 +2399,14 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
-        <color rgb="FF85B739"/>
+        <color rgb="FF85B839"/>
       </left>
       <right style="thin">
-        <color rgb="FF85B739"/>
+        <color rgb="FF85B839"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color rgb="FF85B739"/>
+        <color rgb="FF85B839"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2499,16 +2478,16 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
-        <color rgb="FFFA4808"/>
+        <color rgb="FFF84807"/>
       </left>
       <right style="thin">
-        <color rgb="FFFA4808"/>
+        <color rgb="FFF84807"/>
       </right>
       <top style="thin">
-        <color rgb="FFFA4808"/>
+        <color rgb="FFF84807"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFFA4808"/>
+        <color rgb="FFF84807"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2531,10 +2510,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FFFA4808"/>
+        <color rgb="FFF84807"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFFA4808"/>
+        <color rgb="FFF84807"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2569,16 +2548,16 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
-        <color rgb="FF85B739"/>
+        <color rgb="FF85B839"/>
       </left>
       <right style="thin">
-        <color rgb="FF85B739"/>
+        <color rgb="FF85B839"/>
       </right>
       <top style="thin">
-        <color rgb="FF85B739"/>
+        <color rgb="FF85B839"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF85B739"/>
+        <color rgb="FF85B839"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2591,16 +2570,16 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
-        <color rgb="FFFEE1A3"/>
+        <color rgb="FFFEE1A6"/>
       </left>
       <right style="thin">
-        <color rgb="FFFEE1A3"/>
+        <color rgb="FFFEE1A6"/>
       </right>
       <top style="thin">
-        <color rgb="FFFEE1A3"/>
+        <color rgb="FFFEE1A6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFFEE1A3"/>
+        <color rgb="FFFEE1A6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3413,7 +3392,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="34" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="34" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3577,22 +3556,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="21" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3609,22 +3588,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="23" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="8" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3773,7 +3752,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4357,7 +4336,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="56" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="56" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4461,7 +4440,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4621,7 +4600,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFA4808"/>
+      <rgbColor rgb="FFF84807"/>
       <rgbColor rgb="FF99CC61"/>
       <rgbColor rgb="FF014E52"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -4658,10 +4637,10 @@
       <rgbColor rgb="FF80DEEA"/>
       <rgbColor rgb="FFC5E1A5"/>
       <rgbColor rgb="FFCE93D8"/>
-      <rgbColor rgb="FFFEE1A3"/>
+      <rgbColor rgb="FFFEE1A6"/>
       <rgbColor rgb="FF1D639D"/>
       <rgbColor rgb="FF27C2EF"/>
-      <rgbColor rgb="FF85B739"/>
+      <rgbColor rgb="FF85B839"/>
       <rgbColor rgb="FFFFD63B"/>
       <rgbColor rgb="FFFFA000"/>
       <rgbColor rgb="FFFF6201"/>
@@ -21719,7 +21698,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A146" activeCellId="0" sqref="A146"/>
-      <selection pane="bottomRight" activeCell="H174" activeCellId="0" sqref="H174"/>
+      <selection pane="bottomRight" activeCell="I163" activeCellId="0" sqref="I163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -30765,14 +30744,14 @@
     <tabColor rgb="FF33691E"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK60"/>
+  <dimension ref="A1:AK63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="X27" activeCellId="0" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31052,10 +31031,10 @@
         <v>29</v>
       </c>
       <c r="O7" s="365" t="s">
-        <v>192</v>
+        <v>130</v>
       </c>
       <c r="P7" s="365" t="s">
-        <v>193</v>
+        <v>131</v>
       </c>
       <c r="Q7" s="366" t="s">
         <v>135</v>
@@ -31083,24 +31062,16 @@
       <c r="E8" s="360"/>
       <c r="F8" s="361"/>
       <c r="G8" s="362"/>
-      <c r="H8" s="362" t="s">
-        <v>429</v>
-      </c>
+      <c r="H8" s="362"/>
       <c r="I8" s="362"/>
       <c r="J8" s="362"/>
       <c r="K8" s="362"/>
       <c r="L8" s="362"/>
       <c r="M8" s="363"/>
       <c r="N8" s="364"/>
-      <c r="O8" s="365" t="s">
-        <v>130</v>
-      </c>
-      <c r="P8" s="365" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q8" s="366" t="s">
-        <v>135</v>
-      </c>
+      <c r="O8" s="365"/>
+      <c r="P8" s="365"/>
+      <c r="Q8" s="366"/>
       <c r="R8" s="367"/>
       <c r="S8" s="367"/>
       <c r="T8" s="364"/>
@@ -31125,22 +31096,14 @@
       <c r="F9" s="361"/>
       <c r="G9" s="362"/>
       <c r="H9" s="362"/>
-      <c r="I9" s="362" t="s">
-        <v>430</v>
-      </c>
+      <c r="I9" s="362"/>
       <c r="J9" s="362"/>
       <c r="K9" s="362"/>
       <c r="L9" s="362"/>
       <c r="M9" s="363"/>
-      <c r="N9" s="364" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" s="365" t="s">
-        <v>192</v>
-      </c>
-      <c r="P9" s="365" t="s">
-        <v>193</v>
-      </c>
+      <c r="N9" s="364"/>
+      <c r="O9" s="365"/>
+      <c r="P9" s="365"/>
       <c r="Q9" s="366"/>
       <c r="R9" s="367"/>
       <c r="S9" s="367"/>
@@ -31164,23 +31127,27 @@
       </c>
       <c r="E10" s="360"/>
       <c r="F10" s="361"/>
-      <c r="G10" s="362"/>
+      <c r="G10" s="362" t="s">
+        <v>429</v>
+      </c>
       <c r="H10" s="362"/>
       <c r="I10" s="362"/>
-      <c r="J10" s="362" t="s">
-        <v>431</v>
-      </c>
+      <c r="J10" s="362"/>
       <c r="K10" s="362"/>
       <c r="L10" s="362"/>
       <c r="M10" s="363"/>
-      <c r="N10" s="364"/>
+      <c r="N10" s="364" t="s">
+        <v>29</v>
+      </c>
       <c r="O10" s="365" t="s">
-        <v>130</v>
+        <v>192</v>
       </c>
       <c r="P10" s="365" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q10" s="366"/>
+        <v>193</v>
+      </c>
+      <c r="Q10" s="366" t="s">
+        <v>135</v>
+      </c>
       <c r="R10" s="367"/>
       <c r="S10" s="367"/>
       <c r="T10" s="364"/>
@@ -31204,27 +31171,27 @@
       <c r="E11" s="360"/>
       <c r="F11" s="361"/>
       <c r="G11" s="362"/>
-      <c r="H11" s="362"/>
+      <c r="H11" s="362" t="s">
+        <v>430</v>
+      </c>
       <c r="I11" s="362"/>
       <c r="J11" s="362"/>
-      <c r="K11" s="362" t="s">
-        <v>432</v>
-      </c>
+      <c r="K11" s="362"/>
       <c r="L11" s="362"/>
       <c r="M11" s="363"/>
-      <c r="N11" s="364" t="s">
-        <v>29</v>
-      </c>
-      <c r="O11" s="365"/>
-      <c r="P11" s="365"/>
-      <c r="Q11" s="366"/>
+      <c r="N11" s="364"/>
+      <c r="O11" s="365" t="s">
+        <v>130</v>
+      </c>
+      <c r="P11" s="365" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q11" s="366" t="s">
+        <v>135</v>
+      </c>
       <c r="R11" s="367"/>
-      <c r="S11" s="367" t="s">
-        <v>433</v>
-      </c>
-      <c r="T11" s="364" t="s">
-        <v>135</v>
-      </c>
+      <c r="S11" s="367"/>
+      <c r="T11" s="364"/>
       <c r="U11" s="368"/>
       <c r="V11" s="369"/>
       <c r="W11" s="366"/>
@@ -31246,23 +31213,25 @@
       <c r="F12" s="361"/>
       <c r="G12" s="362"/>
       <c r="H12" s="362"/>
-      <c r="I12" s="362"/>
+      <c r="I12" s="362" t="s">
+        <v>431</v>
+      </c>
       <c r="J12" s="362"/>
-      <c r="K12" s="362" t="s">
-        <v>434</v>
-      </c>
+      <c r="K12" s="362"/>
       <c r="L12" s="362"/>
       <c r="M12" s="363"/>
       <c r="N12" s="364" t="s">
         <v>29</v>
       </c>
-      <c r="O12" s="365"/>
-      <c r="P12" s="365"/>
+      <c r="O12" s="365" t="s">
+        <v>192</v>
+      </c>
+      <c r="P12" s="365" t="s">
+        <v>193</v>
+      </c>
       <c r="Q12" s="366"/>
       <c r="R12" s="367"/>
-      <c r="S12" s="367" t="s">
-        <v>435</v>
-      </c>
+      <c r="S12" s="367"/>
       <c r="T12" s="364"/>
       <c r="U12" s="368"/>
       <c r="V12" s="369"/>
@@ -31284,11 +31253,11 @@
       <c r="E13" s="360"/>
       <c r="F13" s="361"/>
       <c r="G13" s="362"/>
-      <c r="H13" s="362" t="s">
-        <v>429</v>
-      </c>
+      <c r="H13" s="362"/>
       <c r="I13" s="362"/>
-      <c r="J13" s="362"/>
+      <c r="J13" s="362" t="s">
+        <v>432</v>
+      </c>
       <c r="K13" s="362"/>
       <c r="L13" s="362"/>
       <c r="M13" s="363"/>
@@ -31324,26 +31293,26 @@
       <c r="F14" s="361"/>
       <c r="G14" s="362"/>
       <c r="H14" s="362"/>
-      <c r="I14" s="362" t="s">
-        <v>430</v>
-      </c>
+      <c r="I14" s="362"/>
       <c r="J14" s="362"/>
-      <c r="K14" s="362"/>
+      <c r="K14" s="362" t="s">
+        <v>433</v>
+      </c>
       <c r="L14" s="362"/>
       <c r="M14" s="363"/>
       <c r="N14" s="364" t="s">
         <v>29</v>
       </c>
-      <c r="O14" s="365" t="s">
-        <v>192</v>
-      </c>
-      <c r="P14" s="365" t="s">
-        <v>193</v>
-      </c>
+      <c r="O14" s="365"/>
+      <c r="P14" s="365"/>
       <c r="Q14" s="366"/>
       <c r="R14" s="367"/>
-      <c r="S14" s="367"/>
-      <c r="T14" s="364"/>
+      <c r="S14" s="367" t="s">
+        <v>434</v>
+      </c>
+      <c r="T14" s="364" t="s">
+        <v>135</v>
+      </c>
       <c r="U14" s="368"/>
       <c r="V14" s="369"/>
       <c r="W14" s="366"/>
@@ -31366,24 +31335,22 @@
       <c r="G15" s="362"/>
       <c r="H15" s="362"/>
       <c r="I15" s="362"/>
-      <c r="J15" s="362" t="s">
-        <v>431</v>
-      </c>
-      <c r="K15" s="362"/>
+      <c r="J15" s="362"/>
+      <c r="K15" s="362" t="s">
+        <v>435</v>
+      </c>
       <c r="L15" s="362"/>
       <c r="M15" s="363"/>
-      <c r="N15" s="364"/>
-      <c r="O15" s="365" t="s">
-        <v>130</v>
-      </c>
-      <c r="P15" s="365" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q15" s="366" t="s">
-        <v>135</v>
-      </c>
+      <c r="N15" s="364" t="s">
+        <v>29</v>
+      </c>
+      <c r="O15" s="365"/>
+      <c r="P15" s="365"/>
+      <c r="Q15" s="366"/>
       <c r="R15" s="367"/>
-      <c r="S15" s="367"/>
+      <c r="S15" s="367" t="s">
+        <v>436</v>
+      </c>
       <c r="T15" s="364"/>
       <c r="U15" s="368"/>
       <c r="V15" s="369"/>
@@ -31405,27 +31372,25 @@
       <c r="E16" s="360"/>
       <c r="F16" s="361"/>
       <c r="G16" s="362"/>
-      <c r="H16" s="362"/>
+      <c r="H16" s="362" t="s">
+        <v>430</v>
+      </c>
       <c r="I16" s="362"/>
       <c r="J16" s="362"/>
-      <c r="K16" s="362" t="s">
-        <v>432</v>
-      </c>
+      <c r="K16" s="362"/>
       <c r="L16" s="362"/>
       <c r="M16" s="363"/>
-      <c r="N16" s="364" t="s">
-        <v>29</v>
-      </c>
-      <c r="O16" s="365"/>
-      <c r="P16" s="365"/>
+      <c r="N16" s="364"/>
+      <c r="O16" s="365" t="s">
+        <v>130</v>
+      </c>
+      <c r="P16" s="365" t="s">
+        <v>131</v>
+      </c>
       <c r="Q16" s="366"/>
       <c r="R16" s="367"/>
-      <c r="S16" s="367" t="s">
-        <v>133</v>
-      </c>
-      <c r="T16" s="364" t="s">
-        <v>135</v>
-      </c>
+      <c r="S16" s="367"/>
+      <c r="T16" s="364"/>
       <c r="U16" s="368"/>
       <c r="V16" s="369"/>
       <c r="W16" s="366"/>
@@ -31447,23 +31412,25 @@
       <c r="F17" s="361"/>
       <c r="G17" s="362"/>
       <c r="H17" s="362"/>
-      <c r="I17" s="362"/>
+      <c r="I17" s="362" t="s">
+        <v>431</v>
+      </c>
       <c r="J17" s="362"/>
-      <c r="K17" s="362" t="s">
-        <v>434</v>
-      </c>
+      <c r="K17" s="362"/>
       <c r="L17" s="362"/>
       <c r="M17" s="363"/>
       <c r="N17" s="364" t="s">
         <v>29</v>
       </c>
-      <c r="O17" s="365"/>
-      <c r="P17" s="365"/>
+      <c r="O17" s="365" t="s">
+        <v>192</v>
+      </c>
+      <c r="P17" s="365" t="s">
+        <v>193</v>
+      </c>
       <c r="Q17" s="366"/>
       <c r="R17" s="367"/>
-      <c r="S17" s="367" t="s">
-        <v>436</v>
-      </c>
+      <c r="S17" s="367"/>
       <c r="T17" s="364"/>
       <c r="U17" s="368"/>
       <c r="V17" s="369"/>
@@ -31488,7 +31455,7 @@
       <c r="H18" s="362"/>
       <c r="I18" s="362"/>
       <c r="J18" s="362" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="K18" s="362"/>
       <c r="L18" s="362"/>
@@ -31500,7 +31467,9 @@
       <c r="P18" s="365" t="s">
         <v>131</v>
       </c>
-      <c r="Q18" s="366"/>
+      <c r="Q18" s="366" t="s">
+        <v>135</v>
+      </c>
       <c r="R18" s="367"/>
       <c r="S18" s="367"/>
       <c r="T18" s="364"/>
@@ -31528,7 +31497,7 @@
       <c r="I19" s="362"/>
       <c r="J19" s="362"/>
       <c r="K19" s="362" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="L19" s="362"/>
       <c r="M19" s="363"/>
@@ -31540,7 +31509,7 @@
       <c r="Q19" s="366"/>
       <c r="R19" s="367"/>
       <c r="S19" s="367" t="s">
-        <v>437</v>
+        <v>133</v>
       </c>
       <c r="T19" s="364" t="s">
         <v>135</v>
@@ -31569,7 +31538,7 @@
       <c r="I20" s="362"/>
       <c r="J20" s="362"/>
       <c r="K20" s="362" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="L20" s="362"/>
       <c r="M20" s="363"/>
@@ -31581,7 +31550,7 @@
       <c r="Q20" s="366"/>
       <c r="R20" s="367"/>
       <c r="S20" s="367" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="T20" s="364"/>
       <c r="U20" s="368"/>
@@ -31603,27 +31572,23 @@
       </c>
       <c r="E21" s="360"/>
       <c r="F21" s="361"/>
-      <c r="G21" s="362" t="s">
-        <v>439</v>
-      </c>
+      <c r="G21" s="362"/>
       <c r="H21" s="362"/>
       <c r="I21" s="362"/>
-      <c r="J21" s="362"/>
+      <c r="J21" s="362" t="s">
+        <v>432</v>
+      </c>
       <c r="K21" s="362"/>
       <c r="L21" s="362"/>
       <c r="M21" s="363"/>
-      <c r="N21" s="364" t="s">
-        <v>29</v>
-      </c>
+      <c r="N21" s="364"/>
       <c r="O21" s="365" t="s">
-        <v>192</v>
+        <v>130</v>
       </c>
       <c r="P21" s="365" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q21" s="366" t="s">
-        <v>135</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="Q21" s="366"/>
       <c r="R21" s="367"/>
       <c r="S21" s="367"/>
       <c r="T21" s="364"/>
@@ -31647,25 +31612,27 @@
       <c r="E22" s="360"/>
       <c r="F22" s="361"/>
       <c r="G22" s="362"/>
-      <c r="H22" s="362" t="s">
-        <v>440</v>
-      </c>
+      <c r="H22" s="362"/>
       <c r="I22" s="362"/>
       <c r="J22" s="362"/>
-      <c r="K22" s="362"/>
+      <c r="K22" s="362" t="s">
+        <v>433</v>
+      </c>
       <c r="L22" s="362"/>
       <c r="M22" s="363"/>
-      <c r="N22" s="364"/>
-      <c r="O22" s="365" t="s">
-        <v>130</v>
-      </c>
-      <c r="P22" s="365" t="s">
-        <v>131</v>
-      </c>
+      <c r="N22" s="364" t="s">
+        <v>29</v>
+      </c>
+      <c r="O22" s="365"/>
+      <c r="P22" s="365"/>
       <c r="Q22" s="366"/>
       <c r="R22" s="367"/>
-      <c r="S22" s="367"/>
-      <c r="T22" s="364"/>
+      <c r="S22" s="367" t="s">
+        <v>438</v>
+      </c>
+      <c r="T22" s="364" t="s">
+        <v>135</v>
+      </c>
       <c r="U22" s="368"/>
       <c r="V22" s="369"/>
       <c r="W22" s="366"/>
@@ -31687,25 +31654,23 @@
       <c r="F23" s="361"/>
       <c r="G23" s="362"/>
       <c r="H23" s="362"/>
-      <c r="I23" s="362" t="s">
-        <v>430</v>
-      </c>
+      <c r="I23" s="362"/>
       <c r="J23" s="362"/>
-      <c r="K23" s="362"/>
+      <c r="K23" s="362" t="s">
+        <v>435</v>
+      </c>
       <c r="L23" s="362"/>
       <c r="M23" s="363"/>
       <c r="N23" s="364" t="s">
         <v>29</v>
       </c>
-      <c r="O23" s="365" t="s">
-        <v>192</v>
-      </c>
-      <c r="P23" s="365" t="s">
-        <v>193</v>
-      </c>
+      <c r="O23" s="365"/>
+      <c r="P23" s="365"/>
       <c r="Q23" s="366"/>
       <c r="R23" s="367"/>
-      <c r="S23" s="367"/>
+      <c r="S23" s="367" t="s">
+        <v>439</v>
+      </c>
       <c r="T23" s="364"/>
       <c r="U23" s="368"/>
       <c r="V23" s="369"/>
@@ -31726,21 +31691,23 @@
       </c>
       <c r="E24" s="360"/>
       <c r="F24" s="361"/>
-      <c r="G24" s="362"/>
+      <c r="G24" s="362" t="s">
+        <v>440</v>
+      </c>
       <c r="H24" s="362"/>
       <c r="I24" s="362"/>
-      <c r="J24" s="362" t="s">
-        <v>441</v>
-      </c>
+      <c r="J24" s="362"/>
       <c r="K24" s="362"/>
       <c r="L24" s="362"/>
       <c r="M24" s="363"/>
-      <c r="N24" s="364"/>
+      <c r="N24" s="364" t="s">
+        <v>29</v>
+      </c>
       <c r="O24" s="365" t="s">
-        <v>130</v>
+        <v>192</v>
       </c>
       <c r="P24" s="365" t="s">
-        <v>131</v>
+        <v>193</v>
       </c>
       <c r="Q24" s="366" t="s">
         <v>135</v>
@@ -31768,27 +31735,25 @@
       <c r="E25" s="360"/>
       <c r="F25" s="361"/>
       <c r="G25" s="362"/>
-      <c r="H25" s="362"/>
+      <c r="H25" s="362" t="s">
+        <v>441</v>
+      </c>
       <c r="I25" s="362"/>
       <c r="J25" s="362"/>
-      <c r="K25" s="362" t="s">
-        <v>432</v>
-      </c>
+      <c r="K25" s="362"/>
       <c r="L25" s="362"/>
       <c r="M25" s="363"/>
-      <c r="N25" s="364" t="s">
-        <v>29</v>
-      </c>
-      <c r="O25" s="365"/>
-      <c r="P25" s="365"/>
+      <c r="N25" s="364"/>
+      <c r="O25" s="365" t="s">
+        <v>130</v>
+      </c>
+      <c r="P25" s="365" t="s">
+        <v>131</v>
+      </c>
       <c r="Q25" s="366"/>
       <c r="R25" s="367"/>
-      <c r="S25" s="367" t="s">
-        <v>442</v>
-      </c>
-      <c r="T25" s="364" t="s">
-        <v>135</v>
-      </c>
+      <c r="S25" s="367"/>
+      <c r="T25" s="364"/>
       <c r="U25" s="368"/>
       <c r="V25" s="369"/>
       <c r="W25" s="366"/>
@@ -31810,23 +31775,25 @@
       <c r="F26" s="361"/>
       <c r="G26" s="362"/>
       <c r="H26" s="362"/>
-      <c r="I26" s="362"/>
+      <c r="I26" s="362" t="s">
+        <v>431</v>
+      </c>
       <c r="J26" s="362"/>
-      <c r="K26" s="362" t="s">
-        <v>434</v>
-      </c>
+      <c r="K26" s="362"/>
       <c r="L26" s="362"/>
       <c r="M26" s="363"/>
       <c r="N26" s="364" t="s">
         <v>29</v>
       </c>
-      <c r="O26" s="365"/>
-      <c r="P26" s="365"/>
+      <c r="O26" s="365" t="s">
+        <v>192</v>
+      </c>
+      <c r="P26" s="365" t="s">
+        <v>193</v>
+      </c>
       <c r="Q26" s="366"/>
       <c r="R26" s="367"/>
-      <c r="S26" s="367" t="s">
-        <v>443</v>
-      </c>
+      <c r="S26" s="367"/>
       <c r="T26" s="364"/>
       <c r="U26" s="368"/>
       <c r="V26" s="369"/>
@@ -31851,7 +31818,7 @@
       <c r="H27" s="362"/>
       <c r="I27" s="362"/>
       <c r="J27" s="362" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="K27" s="362"/>
       <c r="L27" s="362"/>
@@ -31863,7 +31830,9 @@
       <c r="P27" s="365" t="s">
         <v>131</v>
       </c>
-      <c r="Q27" s="366"/>
+      <c r="Q27" s="366" t="s">
+        <v>135</v>
+      </c>
       <c r="R27" s="367"/>
       <c r="S27" s="367"/>
       <c r="T27" s="364"/>
@@ -31891,7 +31860,7 @@
       <c r="I28" s="362"/>
       <c r="J28" s="362"/>
       <c r="K28" s="362" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="L28" s="362"/>
       <c r="M28" s="363"/>
@@ -31903,7 +31872,7 @@
       <c r="Q28" s="366"/>
       <c r="R28" s="367"/>
       <c r="S28" s="367" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T28" s="364" t="s">
         <v>135</v>
@@ -31932,7 +31901,7 @@
       <c r="I29" s="362"/>
       <c r="J29" s="362"/>
       <c r="K29" s="362" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="L29" s="362"/>
       <c r="M29" s="363"/>
@@ -31944,7 +31913,7 @@
       <c r="Q29" s="366"/>
       <c r="R29" s="367"/>
       <c r="S29" s="367" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T29" s="364"/>
       <c r="U29" s="368"/>
@@ -31966,23 +31935,21 @@
       </c>
       <c r="E30" s="360"/>
       <c r="F30" s="361"/>
-      <c r="G30" s="362" t="s">
-        <v>446</v>
-      </c>
+      <c r="G30" s="362"/>
       <c r="H30" s="362"/>
       <c r="I30" s="362"/>
-      <c r="J30" s="362"/>
+      <c r="J30" s="362" t="s">
+        <v>442</v>
+      </c>
       <c r="K30" s="362"/>
       <c r="L30" s="362"/>
       <c r="M30" s="363"/>
-      <c r="N30" s="364" t="s">
-        <v>29</v>
-      </c>
+      <c r="N30" s="364"/>
       <c r="O30" s="365" t="s">
-        <v>192</v>
+        <v>130</v>
       </c>
       <c r="P30" s="365" t="s">
-        <v>193</v>
+        <v>131</v>
       </c>
       <c r="Q30" s="366"/>
       <c r="R30" s="367"/>
@@ -32008,25 +31975,27 @@
       <c r="E31" s="360"/>
       <c r="F31" s="361"/>
       <c r="G31" s="362"/>
-      <c r="H31" s="362" t="s">
-        <v>447</v>
-      </c>
+      <c r="H31" s="362"/>
       <c r="I31" s="362"/>
       <c r="J31" s="362"/>
-      <c r="K31" s="362"/>
+      <c r="K31" s="362" t="s">
+        <v>433</v>
+      </c>
       <c r="L31" s="362"/>
       <c r="M31" s="363"/>
-      <c r="N31" s="364"/>
-      <c r="O31" s="365" t="s">
-        <v>130</v>
-      </c>
-      <c r="P31" s="365" t="s">
-        <v>131</v>
-      </c>
+      <c r="N31" s="364" t="s">
+        <v>29</v>
+      </c>
+      <c r="O31" s="365"/>
+      <c r="P31" s="365"/>
       <c r="Q31" s="366"/>
       <c r="R31" s="367"/>
-      <c r="S31" s="367"/>
-      <c r="T31" s="364"/>
+      <c r="S31" s="367" t="s">
+        <v>445</v>
+      </c>
+      <c r="T31" s="364" t="s">
+        <v>135</v>
+      </c>
       <c r="U31" s="368"/>
       <c r="V31" s="369"/>
       <c r="W31" s="366"/>
@@ -32048,25 +32017,23 @@
       <c r="F32" s="361"/>
       <c r="G32" s="362"/>
       <c r="H32" s="362"/>
-      <c r="I32" s="362" t="s">
-        <v>430</v>
-      </c>
+      <c r="I32" s="362"/>
       <c r="J32" s="362"/>
-      <c r="K32" s="362"/>
+      <c r="K32" s="362" t="s">
+        <v>435</v>
+      </c>
       <c r="L32" s="362"/>
       <c r="M32" s="363"/>
       <c r="N32" s="364" t="s">
         <v>29</v>
       </c>
-      <c r="O32" s="365" t="s">
-        <v>192</v>
-      </c>
-      <c r="P32" s="365" t="s">
-        <v>193</v>
-      </c>
+      <c r="O32" s="365"/>
+      <c r="P32" s="365"/>
       <c r="Q32" s="366"/>
       <c r="R32" s="367"/>
-      <c r="S32" s="367"/>
+      <c r="S32" s="367" t="s">
+        <v>446</v>
+      </c>
       <c r="T32" s="364"/>
       <c r="U32" s="368"/>
       <c r="V32" s="369"/>
@@ -32087,25 +32054,25 @@
       </c>
       <c r="E33" s="360"/>
       <c r="F33" s="361"/>
-      <c r="G33" s="362"/>
+      <c r="G33" s="362" t="s">
+        <v>447</v>
+      </c>
       <c r="H33" s="362"/>
       <c r="I33" s="362"/>
-      <c r="J33" s="362" t="s">
-        <v>448</v>
-      </c>
+      <c r="J33" s="362"/>
       <c r="K33" s="362"/>
       <c r="L33" s="362"/>
       <c r="M33" s="363"/>
-      <c r="N33" s="364"/>
+      <c r="N33" s="364" t="s">
+        <v>29</v>
+      </c>
       <c r="O33" s="365" t="s">
-        <v>130</v>
+        <v>192</v>
       </c>
       <c r="P33" s="365" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q33" s="366" t="s">
-        <v>135</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="Q33" s="366"/>
       <c r="R33" s="367"/>
       <c r="S33" s="367"/>
       <c r="T33" s="364"/>
@@ -32129,27 +32096,25 @@
       <c r="E34" s="360"/>
       <c r="F34" s="361"/>
       <c r="G34" s="362"/>
-      <c r="H34" s="362"/>
+      <c r="H34" s="362" t="s">
+        <v>448</v>
+      </c>
       <c r="I34" s="362"/>
       <c r="J34" s="362"/>
-      <c r="K34" s="362" t="s">
-        <v>432</v>
-      </c>
+      <c r="K34" s="362"/>
       <c r="L34" s="362"/>
       <c r="M34" s="363"/>
-      <c r="N34" s="364" t="s">
-        <v>29</v>
-      </c>
-      <c r="O34" s="365"/>
-      <c r="P34" s="365"/>
+      <c r="N34" s="364"/>
+      <c r="O34" s="365" t="s">
+        <v>130</v>
+      </c>
+      <c r="P34" s="365" t="s">
+        <v>131</v>
+      </c>
       <c r="Q34" s="366"/>
       <c r="R34" s="367"/>
-      <c r="S34" s="367" t="s">
-        <v>142</v>
-      </c>
-      <c r="T34" s="364" t="s">
-        <v>135</v>
-      </c>
+      <c r="S34" s="367"/>
+      <c r="T34" s="364"/>
       <c r="U34" s="368"/>
       <c r="V34" s="369"/>
       <c r="W34" s="366"/>
@@ -32171,23 +32136,25 @@
       <c r="F35" s="361"/>
       <c r="G35" s="362"/>
       <c r="H35" s="362"/>
-      <c r="I35" s="362"/>
+      <c r="I35" s="362" t="s">
+        <v>431</v>
+      </c>
       <c r="J35" s="362"/>
-      <c r="K35" s="362" t="s">
-        <v>434</v>
-      </c>
+      <c r="K35" s="362"/>
       <c r="L35" s="362"/>
       <c r="M35" s="363"/>
       <c r="N35" s="364" t="s">
         <v>29</v>
       </c>
-      <c r="O35" s="365"/>
-      <c r="P35" s="365"/>
+      <c r="O35" s="365" t="s">
+        <v>192</v>
+      </c>
+      <c r="P35" s="365" t="s">
+        <v>193</v>
+      </c>
       <c r="Q35" s="366"/>
       <c r="R35" s="367"/>
-      <c r="S35" s="367" t="s">
-        <v>143</v>
-      </c>
+      <c r="S35" s="367"/>
       <c r="T35" s="364"/>
       <c r="U35" s="368"/>
       <c r="V35" s="369"/>
@@ -32212,7 +32179,7 @@
       <c r="H36" s="362"/>
       <c r="I36" s="362"/>
       <c r="J36" s="362" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="K36" s="362"/>
       <c r="L36" s="362"/>
@@ -32224,7 +32191,9 @@
       <c r="P36" s="365" t="s">
         <v>131</v>
       </c>
-      <c r="Q36" s="366"/>
+      <c r="Q36" s="366" t="s">
+        <v>135</v>
+      </c>
       <c r="R36" s="367"/>
       <c r="S36" s="367"/>
       <c r="T36" s="364"/>
@@ -32252,7 +32221,7 @@
       <c r="I37" s="362"/>
       <c r="J37" s="362"/>
       <c r="K37" s="362" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="L37" s="362"/>
       <c r="M37" s="363"/>
@@ -32264,7 +32233,7 @@
       <c r="Q37" s="366"/>
       <c r="R37" s="367"/>
       <c r="S37" s="367" t="s">
-        <v>449</v>
+        <v>142</v>
       </c>
       <c r="T37" s="364" t="s">
         <v>135</v>
@@ -32293,7 +32262,7 @@
       <c r="I38" s="362"/>
       <c r="J38" s="362"/>
       <c r="K38" s="362" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="L38" s="362"/>
       <c r="M38" s="363"/>
@@ -32305,7 +32274,7 @@
       <c r="Q38" s="366"/>
       <c r="R38" s="367"/>
       <c r="S38" s="367" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="T38" s="364"/>
       <c r="U38" s="368"/>
@@ -32317,73 +32286,80 @@
       <c r="AK38" s="290"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="73" t="n">
-        <f aca="false">VINE!$A$40</f>
-        <v>36</v>
-      </c>
-      <c r="B39" s="74" t="s">
-        <v>450</v>
-      </c>
-      <c r="C39" s="75"/>
-      <c r="D39" s="75"/>
-      <c r="E39" s="370"/>
-      <c r="F39" s="75"/>
-      <c r="G39" s="75"/>
-      <c r="H39" s="75"/>
-      <c r="I39" s="75"/>
-      <c r="J39" s="75"/>
-      <c r="K39" s="75"/>
-      <c r="L39" s="75"/>
-      <c r="M39" s="75"/>
-      <c r="N39" s="75"/>
-      <c r="O39" s="75"/>
-      <c r="P39" s="75"/>
-      <c r="Q39" s="75"/>
-      <c r="R39" s="75"/>
-      <c r="S39" s="75"/>
-      <c r="T39" s="75"/>
-      <c r="U39" s="75"/>
-      <c r="V39" s="75"/>
-      <c r="W39" s="75"/>
+      <c r="A39" s="357"/>
+      <c r="B39" s="357"/>
+      <c r="C39" s="358" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="359" t="s">
+        <v>128</v>
+      </c>
+      <c r="E39" s="360"/>
+      <c r="F39" s="361"/>
+      <c r="G39" s="362"/>
+      <c r="H39" s="362"/>
+      <c r="I39" s="362"/>
+      <c r="J39" s="362" t="s">
+        <v>449</v>
+      </c>
+      <c r="K39" s="362"/>
+      <c r="L39" s="362"/>
+      <c r="M39" s="363"/>
+      <c r="N39" s="364"/>
+      <c r="O39" s="365" t="s">
+        <v>130</v>
+      </c>
+      <c r="P39" s="365" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q39" s="366"/>
+      <c r="R39" s="367"/>
+      <c r="S39" s="367"/>
+      <c r="T39" s="364"/>
+      <c r="U39" s="368"/>
+      <c r="V39" s="369"/>
+      <c r="W39" s="366"/>
       <c r="X39" s="68"/>
       <c r="Y39" s="293"/>
       <c r="AJ39" s="290"/>
       <c r="AK39" s="290"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="302"/>
-      <c r="B40" s="302"/>
-      <c r="C40" s="303" t="s">
-        <v>127</v>
-      </c>
-      <c r="D40" s="304" t="s">
-        <v>128</v>
-      </c>
-      <c r="E40" s="356"/>
-      <c r="F40" s="306" t="s">
-        <v>425</v>
-      </c>
-      <c r="G40" s="305"/>
-      <c r="H40" s="305"/>
-      <c r="I40" s="305"/>
-      <c r="J40" s="305"/>
-      <c r="K40" s="305"/>
-      <c r="L40" s="305"/>
-      <c r="M40" s="307"/>
-      <c r="N40" s="308"/>
-      <c r="O40" s="309" t="s">
-        <v>225</v>
-      </c>
-      <c r="P40" s="309" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q40" s="310"/>
-      <c r="R40" s="311"/>
-      <c r="S40" s="311"/>
-      <c r="T40" s="308"/>
-      <c r="U40" s="312"/>
-      <c r="V40" s="313"/>
-      <c r="W40" s="310"/>
+      <c r="A40" s="357"/>
+      <c r="B40" s="357"/>
+      <c r="C40" s="358" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="359" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" s="360"/>
+      <c r="F40" s="361"/>
+      <c r="G40" s="362"/>
+      <c r="H40" s="362"/>
+      <c r="I40" s="362"/>
+      <c r="J40" s="362"/>
+      <c r="K40" s="362" t="s">
+        <v>433</v>
+      </c>
+      <c r="L40" s="362"/>
+      <c r="M40" s="363"/>
+      <c r="N40" s="364" t="s">
+        <v>29</v>
+      </c>
+      <c r="O40" s="365"/>
+      <c r="P40" s="365"/>
+      <c r="Q40" s="366"/>
+      <c r="R40" s="367"/>
+      <c r="S40" s="367" t="s">
+        <v>450</v>
+      </c>
+      <c r="T40" s="364" t="s">
+        <v>135</v>
+      </c>
+      <c r="U40" s="368"/>
+      <c r="V40" s="369"/>
+      <c r="W40" s="366"/>
       <c r="X40" s="68"/>
       <c r="Y40" s="293"/>
       <c r="AJ40" s="290"/>
@@ -32400,21 +32376,25 @@
       </c>
       <c r="E41" s="360"/>
       <c r="F41" s="361"/>
-      <c r="G41" s="362" t="s">
-        <v>451</v>
-      </c>
+      <c r="G41" s="362"/>
       <c r="H41" s="362"/>
       <c r="I41" s="362"/>
       <c r="J41" s="362"/>
-      <c r="K41" s="362"/>
+      <c r="K41" s="362" t="s">
+        <v>435</v>
+      </c>
       <c r="L41" s="362"/>
       <c r="M41" s="363"/>
-      <c r="N41" s="364"/>
+      <c r="N41" s="364" t="s">
+        <v>29</v>
+      </c>
       <c r="O41" s="365"/>
       <c r="P41" s="365"/>
       <c r="Q41" s="366"/>
       <c r="R41" s="367"/>
-      <c r="S41" s="367"/>
+      <c r="S41" s="367" t="s">
+        <v>141</v>
+      </c>
       <c r="T41" s="364"/>
       <c r="U41" s="368"/>
       <c r="V41" s="369"/>
@@ -32424,97 +32404,187 @@
       <c r="AJ41" s="290"/>
       <c r="AK41" s="290"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="68"/>
-      <c r="B42" s="68"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="68"/>
-      <c r="J42" s="68"/>
-      <c r="K42" s="68"/>
-      <c r="L42" s="68"/>
-      <c r="M42" s="68"/>
-      <c r="N42" s="68"/>
-      <c r="O42" s="68"/>
-      <c r="P42" s="68"/>
-      <c r="Q42" s="68"/>
-      <c r="R42" s="68"/>
-      <c r="S42" s="68"/>
-      <c r="T42" s="68"/>
-      <c r="U42" s="68"/>
-      <c r="V42" s="68"/>
-      <c r="W42" s="68"/>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="73" t="n">
+        <f aca="false">VINE!$A$40</f>
+        <v>36</v>
+      </c>
+      <c r="B42" s="74" t="s">
+        <v>451</v>
+      </c>
+      <c r="C42" s="75"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="370"/>
+      <c r="F42" s="75"/>
+      <c r="G42" s="75"/>
+      <c r="H42" s="75"/>
+      <c r="I42" s="75"/>
+      <c r="J42" s="75"/>
+      <c r="K42" s="75"/>
+      <c r="L42" s="75"/>
+      <c r="M42" s="75"/>
+      <c r="N42" s="75"/>
+      <c r="O42" s="75"/>
+      <c r="P42" s="75"/>
+      <c r="Q42" s="75"/>
+      <c r="R42" s="75"/>
+      <c r="S42" s="75"/>
+      <c r="T42" s="75"/>
+      <c r="U42" s="75"/>
+      <c r="V42" s="75"/>
+      <c r="W42" s="75"/>
       <c r="X42" s="68"/>
       <c r="Y42" s="293"/>
-      <c r="AE42" s="290"/>
-      <c r="AF42" s="290"/>
       <c r="AJ42" s="290"/>
       <c r="AK42" s="290"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="293"/>
-      <c r="B43" s="293"/>
-      <c r="C43" s="352"/>
-      <c r="D43" s="352"/>
-      <c r="E43" s="352"/>
-      <c r="F43" s="353" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" s="353" t="n">
-        <v>1</v>
-      </c>
-      <c r="H43" s="353" t="n">
-        <v>2</v>
-      </c>
-      <c r="I43" s="353" t="n">
-        <v>3</v>
-      </c>
-      <c r="J43" s="353" t="n">
-        <v>4</v>
-      </c>
-      <c r="K43" s="353" t="n">
-        <v>5</v>
-      </c>
-      <c r="L43" s="353" t="n">
-        <v>6</v>
-      </c>
-      <c r="M43" s="353" t="n">
-        <v>7</v>
-      </c>
-      <c r="N43" s="354"/>
-      <c r="O43" s="355"/>
-      <c r="P43" s="355"/>
-      <c r="Q43" s="354"/>
-      <c r="R43" s="352"/>
-      <c r="S43" s="293"/>
-      <c r="T43" s="355"/>
-      <c r="U43" s="355"/>
-      <c r="V43" s="355"/>
-      <c r="W43" s="355"/>
-      <c r="X43" s="293"/>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="302"/>
+      <c r="B43" s="302"/>
+      <c r="C43" s="303" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="304" t="s">
+        <v>128</v>
+      </c>
+      <c r="E43" s="356"/>
+      <c r="F43" s="306" t="s">
+        <v>425</v>
+      </c>
+      <c r="G43" s="305"/>
+      <c r="H43" s="305"/>
+      <c r="I43" s="305"/>
+      <c r="J43" s="305"/>
+      <c r="K43" s="305"/>
+      <c r="L43" s="305"/>
+      <c r="M43" s="307"/>
+      <c r="N43" s="308"/>
+      <c r="O43" s="309" t="s">
+        <v>225</v>
+      </c>
+      <c r="P43" s="309" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q43" s="310"/>
+      <c r="R43" s="311"/>
+      <c r="S43" s="311"/>
+      <c r="T43" s="308"/>
+      <c r="U43" s="312"/>
+      <c r="V43" s="313"/>
+      <c r="W43" s="310"/>
+      <c r="X43" s="68"/>
       <c r="Y43" s="293"/>
-      <c r="AE43" s="290"/>
-      <c r="AF43" s="290"/>
       <c r="AJ43" s="290"/>
       <c r="AK43" s="290"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AE44" s="290"/>
-      <c r="AF44" s="290"/>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="357"/>
+      <c r="B44" s="357"/>
+      <c r="C44" s="358" t="s">
+        <v>127</v>
+      </c>
+      <c r="D44" s="359" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" s="360"/>
+      <c r="F44" s="361"/>
+      <c r="G44" s="362" t="s">
+        <v>452</v>
+      </c>
+      <c r="H44" s="362"/>
+      <c r="I44" s="362"/>
+      <c r="J44" s="362"/>
+      <c r="K44" s="362"/>
+      <c r="L44" s="362"/>
+      <c r="M44" s="363"/>
+      <c r="N44" s="364"/>
+      <c r="O44" s="365"/>
+      <c r="P44" s="365"/>
+      <c r="Q44" s="366"/>
+      <c r="R44" s="367"/>
+      <c r="S44" s="367"/>
+      <c r="T44" s="364"/>
+      <c r="U44" s="368"/>
+      <c r="V44" s="369"/>
+      <c r="W44" s="366"/>
+      <c r="X44" s="68"/>
+      <c r="Y44" s="293"/>
       <c r="AJ44" s="290"/>
       <c r="AK44" s="290"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="68"/>
+      <c r="B45" s="68"/>
+      <c r="C45" s="68"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="68"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="68"/>
+      <c r="H45" s="68"/>
+      <c r="I45" s="68"/>
+      <c r="J45" s="68"/>
+      <c r="K45" s="68"/>
+      <c r="L45" s="68"/>
+      <c r="M45" s="68"/>
+      <c r="N45" s="68"/>
+      <c r="O45" s="68"/>
+      <c r="P45" s="68"/>
+      <c r="Q45" s="68"/>
+      <c r="R45" s="68"/>
+      <c r="S45" s="68"/>
+      <c r="T45" s="68"/>
+      <c r="U45" s="68"/>
+      <c r="V45" s="68"/>
+      <c r="W45" s="68"/>
+      <c r="X45" s="68"/>
+      <c r="Y45" s="293"/>
       <c r="AE45" s="290"/>
       <c r="AF45" s="290"/>
       <c r="AJ45" s="290"/>
       <c r="AK45" s="290"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="293"/>
+      <c r="B46" s="293"/>
+      <c r="C46" s="352"/>
+      <c r="D46" s="352"/>
+      <c r="E46" s="352"/>
+      <c r="F46" s="353" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="353" t="n">
+        <v>1</v>
+      </c>
+      <c r="H46" s="353" t="n">
+        <v>2</v>
+      </c>
+      <c r="I46" s="353" t="n">
+        <v>3</v>
+      </c>
+      <c r="J46" s="353" t="n">
+        <v>4</v>
+      </c>
+      <c r="K46" s="353" t="n">
+        <v>5</v>
+      </c>
+      <c r="L46" s="353" t="n">
+        <v>6</v>
+      </c>
+      <c r="M46" s="353" t="n">
+        <v>7</v>
+      </c>
+      <c r="N46" s="354"/>
+      <c r="O46" s="355"/>
+      <c r="P46" s="355"/>
+      <c r="Q46" s="354"/>
+      <c r="R46" s="352"/>
+      <c r="S46" s="293"/>
+      <c r="T46" s="355"/>
+      <c r="U46" s="355"/>
+      <c r="V46" s="355"/>
+      <c r="W46" s="355"/>
+      <c r="X46" s="293"/>
+      <c r="Y46" s="293"/>
       <c r="AE46" s="290"/>
       <c r="AF46" s="290"/>
       <c r="AJ46" s="290"/>
@@ -32603,6 +32673,24 @@
       <c r="AF60" s="290"/>
       <c r="AJ60" s="290"/>
       <c r="AK60" s="290"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE61" s="290"/>
+      <c r="AF61" s="290"/>
+      <c r="AJ61" s="290"/>
+      <c r="AK61" s="290"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE62" s="290"/>
+      <c r="AF62" s="290"/>
+      <c r="AJ62" s="290"/>
+      <c r="AK62" s="290"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AE63" s="290"/>
+      <c r="AF63" s="290"/>
+      <c r="AJ63" s="290"/>
+      <c r="AK63" s="290"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -32696,7 +32784,7 @@
       </c>
       <c r="D1" s="372"/>
       <c r="E1" s="373" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F1" s="373"/>
       <c r="G1" s="373"/>
@@ -32707,7 +32795,7 @@
       <c r="L1" s="373"/>
       <c r="M1" s="373"/>
       <c r="N1" s="373" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="O1" s="373"/>
       <c r="P1" s="373"/>
@@ -32716,7 +32804,7 @@
       <c r="S1" s="373"/>
       <c r="T1" s="373"/>
       <c r="U1" s="374" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="V1" s="375" t="s">
         <v>111</v>
@@ -32743,7 +32831,7 @@
       <c r="AN1" s="276"/>
       <c r="AO1" s="276"/>
       <c r="AP1" s="376" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AQ1" s="376"/>
       <c r="AR1" s="376"/>
@@ -32767,7 +32855,7 @@
         <v>116</v>
       </c>
       <c r="E2" s="380" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F2" s="380"/>
       <c r="G2" s="380"/>
@@ -32778,20 +32866,20 @@
       <c r="L2" s="380"/>
       <c r="M2" s="380"/>
       <c r="N2" s="380" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="O2" s="380"/>
       <c r="P2" s="373" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="Q2" s="373"/>
       <c r="R2" s="373"/>
       <c r="S2" s="380" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="T2" s="380"/>
       <c r="U2" s="376" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="V2" s="375" t="s">
         <v>117</v>
@@ -32849,7 +32937,7 @@
       <c r="L3" s="373"/>
       <c r="M3" s="373"/>
       <c r="N3" s="382" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="O3" s="382"/>
       <c r="P3" s="373" t="s">
@@ -32859,10 +32947,10 @@
         <v>121</v>
       </c>
       <c r="R3" s="373" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="S3" s="382" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="T3" s="382"/>
       <c r="U3" s="374" t="s">
@@ -33002,7 +33090,7 @@
         <v>42</v>
       </c>
       <c r="B5" s="389" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C5" s="390"/>
       <c r="D5" s="390"/>
@@ -33059,7 +33147,7 @@
         <v>127</v>
       </c>
       <c r="D6" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E6" s="400"/>
       <c r="F6" s="400"/>
@@ -33080,7 +33168,7 @@
       <c r="U6" s="405"/>
       <c r="V6" s="406"/>
       <c r="W6" s="407" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="X6" s="407"/>
       <c r="Y6" s="407"/>
@@ -33092,10 +33180,10 @@
       <c r="AE6" s="407"/>
       <c r="AF6" s="408"/>
       <c r="AG6" s="409" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AH6" s="410" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AI6" s="411"/>
       <c r="AJ6" s="412"/>
@@ -33120,7 +33208,7 @@
         <v>127</v>
       </c>
       <c r="D7" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E7" s="400"/>
       <c r="F7" s="400"/>
@@ -33161,7 +33249,7 @@
       <c r="AI7" s="411"/>
       <c r="AJ7" s="412"/>
       <c r="AK7" s="210" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AL7" s="413"/>
       <c r="AM7" s="414"/>
@@ -33183,7 +33271,7 @@
         <v>127</v>
       </c>
       <c r="D8" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E8" s="400"/>
       <c r="F8" s="400"/>
@@ -33224,7 +33312,7 @@
       <c r="AI8" s="411"/>
       <c r="AJ8" s="412"/>
       <c r="AK8" s="210" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="AL8" s="413"/>
       <c r="AM8" s="414"/>
@@ -33246,10 +33334,10 @@
         <v>127</v>
       </c>
       <c r="D9" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E9" s="419" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F9" s="419"/>
       <c r="G9" s="419"/>
@@ -33260,10 +33348,10 @@
       <c r="L9" s="419"/>
       <c r="M9" s="419"/>
       <c r="N9" s="401" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="O9" s="402" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P9" s="420"/>
       <c r="Q9" s="421"/>
@@ -33309,7 +33397,7 @@
         <v>127</v>
       </c>
       <c r="D10" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E10" s="422" t="s">
         <v>105</v>
@@ -33323,25 +33411,25 @@
       <c r="L10" s="422"/>
       <c r="M10" s="422"/>
       <c r="N10" s="401" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="O10" s="402" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P10" s="420" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="Q10" s="421" t="s">
         <v>190</v>
       </c>
       <c r="R10" s="420" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="S10" s="401" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="T10" s="402" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="U10" s="405"/>
       <c r="V10" s="406"/>
@@ -33380,11 +33468,11 @@
         <v>127</v>
       </c>
       <c r="D11" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E11" s="400"/>
       <c r="F11" s="422" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G11" s="422"/>
       <c r="H11" s="422"/>
@@ -33394,19 +33482,19 @@
       <c r="L11" s="422"/>
       <c r="M11" s="422"/>
       <c r="N11" s="401" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="O11" s="402" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P11" s="403"/>
       <c r="Q11" s="404"/>
       <c r="R11" s="403"/>
       <c r="S11" s="401" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="T11" s="402" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="U11" s="405"/>
       <c r="V11" s="406"/>
@@ -33445,12 +33533,12 @@
         <v>127</v>
       </c>
       <c r="D12" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E12" s="400"/>
       <c r="F12" s="400"/>
       <c r="G12" s="422" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H12" s="422"/>
       <c r="I12" s="422"/>
@@ -33459,19 +33547,19 @@
       <c r="L12" s="422"/>
       <c r="M12" s="422"/>
       <c r="N12" s="401" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="O12" s="402" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P12" s="403"/>
       <c r="Q12" s="404"/>
       <c r="R12" s="403"/>
       <c r="S12" s="401" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="T12" s="402" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="U12" s="405"/>
       <c r="V12" s="406"/>
@@ -33510,13 +33598,13 @@
         <v>127</v>
       </c>
       <c r="D13" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E13" s="400"/>
       <c r="F13" s="400"/>
       <c r="G13" s="423"/>
       <c r="H13" s="423" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="I13" s="423"/>
       <c r="J13" s="423"/>
@@ -33531,7 +33619,7 @@
       <c r="S13" s="401"/>
       <c r="T13" s="402"/>
       <c r="U13" s="424" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="V13" s="406"/>
       <c r="W13" s="418"/>
@@ -33569,7 +33657,7 @@
         <v>127</v>
       </c>
       <c r="D14" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E14" s="400"/>
       <c r="F14" s="400"/>
@@ -33592,7 +33680,7 @@
       <c r="W14" s="418"/>
       <c r="X14" s="418"/>
       <c r="Y14" s="407" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="Z14" s="407"/>
       <c r="AA14" s="407"/>
@@ -33602,10 +33690,10 @@
       <c r="AE14" s="407"/>
       <c r="AF14" s="408"/>
       <c r="AG14" s="409" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AH14" s="410" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AI14" s="411"/>
       <c r="AJ14" s="412"/>
@@ -33630,7 +33718,7 @@
         <v>127</v>
       </c>
       <c r="D15" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E15" s="400"/>
       <c r="F15" s="400"/>
@@ -33656,7 +33744,7 @@
       <c r="X15" s="418"/>
       <c r="Y15" s="418"/>
       <c r="Z15" s="407" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AA15" s="407"/>
       <c r="AB15" s="407"/>
@@ -33693,7 +33781,7 @@
         <v>127</v>
       </c>
       <c r="D16" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E16" s="400"/>
       <c r="F16" s="400"/>
@@ -33718,7 +33806,7 @@
       <c r="Y16" s="418"/>
       <c r="Z16" s="418"/>
       <c r="AA16" s="407" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AB16" s="407"/>
       <c r="AC16" s="407"/>
@@ -33750,7 +33838,7 @@
         <v>127</v>
       </c>
       <c r="D17" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E17" s="400"/>
       <c r="F17" s="400"/>
@@ -33774,7 +33862,7 @@
       <c r="X17" s="418"/>
       <c r="Y17" s="418"/>
       <c r="Z17" s="407" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AA17" s="407"/>
       <c r="AB17" s="407"/>
@@ -33811,7 +33899,7 @@
         <v>127</v>
       </c>
       <c r="D18" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E18" s="400"/>
       <c r="F18" s="400"/>
@@ -33838,7 +33926,7 @@
       <c r="Y18" s="418"/>
       <c r="Z18" s="418"/>
       <c r="AA18" s="407" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="AB18" s="407"/>
       <c r="AC18" s="407"/>
@@ -33874,7 +33962,7 @@
         <v>127</v>
       </c>
       <c r="D19" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E19" s="400"/>
       <c r="F19" s="400"/>
@@ -33902,7 +33990,7 @@
       <c r="Z19" s="418"/>
       <c r="AA19" s="418"/>
       <c r="AB19" s="407" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="AC19" s="407"/>
       <c r="AD19" s="407"/>
@@ -33915,7 +34003,7 @@
         <v>234</v>
       </c>
       <c r="AK19" s="210" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AL19" s="413"/>
       <c r="AM19" s="414"/>
@@ -33937,7 +34025,7 @@
         <v>127</v>
       </c>
       <c r="D20" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E20" s="400"/>
       <c r="F20" s="400"/>
@@ -33962,7 +34050,7 @@
       <c r="Y20" s="418"/>
       <c r="Z20" s="418"/>
       <c r="AA20" s="407" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AB20" s="407"/>
       <c r="AC20" s="407"/>
@@ -33970,10 +34058,10 @@
       <c r="AE20" s="407"/>
       <c r="AF20" s="408"/>
       <c r="AG20" s="425" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AH20" s="426" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AI20" s="411"/>
       <c r="AJ20" s="412"/>
@@ -33998,7 +34086,7 @@
         <v>127</v>
       </c>
       <c r="D21" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E21" s="400"/>
       <c r="F21" s="400"/>
@@ -34006,16 +34094,16 @@
       <c r="H21" s="400"/>
       <c r="I21" s="400"/>
       <c r="J21" s="422" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="K21" s="422"/>
       <c r="L21" s="422"/>
       <c r="M21" s="422"/>
       <c r="N21" s="427" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="O21" s="428" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P21" s="32"/>
       <c r="Q21" s="429"/>
@@ -34059,7 +34147,7 @@
         <v>127</v>
       </c>
       <c r="D22" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E22" s="400"/>
       <c r="F22" s="400"/>
@@ -34086,16 +34174,16 @@
       <c r="AA22" s="434"/>
       <c r="AB22" s="434"/>
       <c r="AC22" s="407" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="AD22" s="407"/>
       <c r="AE22" s="407"/>
       <c r="AF22" s="435"/>
       <c r="AG22" s="436" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AH22" s="437" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AI22" s="438"/>
       <c r="AJ22" s="439"/>
@@ -34120,7 +34208,7 @@
         <v>127</v>
       </c>
       <c r="D23" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E23" s="400"/>
       <c r="F23" s="400"/>
@@ -34150,7 +34238,7 @@
       <c r="AB23" s="434"/>
       <c r="AC23" s="434"/>
       <c r="AD23" s="407" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="AE23" s="407"/>
       <c r="AF23" s="435"/>
@@ -34183,7 +34271,7 @@
         <v>127</v>
       </c>
       <c r="D24" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E24" s="400"/>
       <c r="F24" s="400"/>
@@ -34214,7 +34302,7 @@
       <c r="AC24" s="434"/>
       <c r="AD24" s="434"/>
       <c r="AE24" s="407" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="AF24" s="435"/>
       <c r="AG24" s="436"/>
@@ -34224,7 +34312,7 @@
         <v>234</v>
       </c>
       <c r="AK24" s="271" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="AL24" s="413"/>
       <c r="AM24" s="440"/>
@@ -34246,7 +34334,7 @@
         <v>127</v>
       </c>
       <c r="D25" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E25" s="400"/>
       <c r="F25" s="400"/>
@@ -34274,15 +34362,15 @@
       <c r="AB25" s="434"/>
       <c r="AC25" s="434"/>
       <c r="AD25" s="407" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AE25" s="407"/>
       <c r="AF25" s="435"/>
       <c r="AG25" s="425" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AH25" s="426" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AI25" s="438"/>
       <c r="AJ25" s="439"/>
@@ -34307,7 +34395,7 @@
         <v>127</v>
       </c>
       <c r="D26" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E26" s="400"/>
       <c r="F26" s="400"/>
@@ -34318,18 +34406,18 @@
       <c r="K26" s="443"/>
       <c r="L26" s="443"/>
       <c r="M26" s="446" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="N26" s="447"/>
       <c r="O26" s="448"/>
       <c r="P26" s="420" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="Q26" s="421" t="s">
         <v>190</v>
       </c>
       <c r="R26" s="420" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="S26" s="430"/>
       <c r="T26" s="431"/>
@@ -34370,7 +34458,7 @@
         <v>127</v>
       </c>
       <c r="D27" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E27" s="400"/>
       <c r="F27" s="400"/>
@@ -34393,7 +34481,7 @@
       <c r="W27" s="418"/>
       <c r="X27" s="418"/>
       <c r="Y27" s="407" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="Z27" s="407"/>
       <c r="AA27" s="407"/>
@@ -34403,10 +34491,10 @@
       <c r="AE27" s="407"/>
       <c r="AF27" s="408"/>
       <c r="AG27" s="409" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AH27" s="410" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AI27" s="411"/>
       <c r="AJ27" s="412"/>
@@ -34431,7 +34519,7 @@
         <v>127</v>
       </c>
       <c r="D28" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E28" s="400"/>
       <c r="F28" s="400"/>
@@ -34457,7 +34545,7 @@
       <c r="X28" s="418"/>
       <c r="Y28" s="418"/>
       <c r="Z28" s="407" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="AA28" s="407"/>
       <c r="AB28" s="407"/>
@@ -34494,7 +34582,7 @@
         <v>127</v>
       </c>
       <c r="D29" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E29" s="400"/>
       <c r="F29" s="400"/>
@@ -34519,7 +34607,7 @@
       <c r="Y29" s="418"/>
       <c r="Z29" s="418"/>
       <c r="AA29" s="407" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="AB29" s="407"/>
       <c r="AC29" s="407"/>
@@ -34551,7 +34639,7 @@
         <v>127</v>
       </c>
       <c r="D30" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E30" s="400"/>
       <c r="F30" s="400"/>
@@ -34575,7 +34663,7 @@
       <c r="X30" s="418"/>
       <c r="Y30" s="418"/>
       <c r="Z30" s="407" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="AA30" s="407"/>
       <c r="AB30" s="407"/>
@@ -34612,7 +34700,7 @@
         <v>127</v>
       </c>
       <c r="D31" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E31" s="400"/>
       <c r="F31" s="400"/>
@@ -34639,7 +34727,7 @@
       <c r="Y31" s="418"/>
       <c r="Z31" s="418"/>
       <c r="AA31" s="407" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="AB31" s="407"/>
       <c r="AC31" s="407"/>
@@ -34675,7 +34763,7 @@
         <v>127</v>
       </c>
       <c r="D32" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E32" s="400"/>
       <c r="F32" s="400"/>
@@ -34703,7 +34791,7 @@
       <c r="Z32" s="418"/>
       <c r="AA32" s="418"/>
       <c r="AB32" s="407" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="AC32" s="407"/>
       <c r="AD32" s="407"/>
@@ -34716,7 +34804,7 @@
         <v>234</v>
       </c>
       <c r="AK32" s="210" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="AL32" s="413"/>
       <c r="AM32" s="414"/>
@@ -34738,7 +34826,7 @@
         <v>127</v>
       </c>
       <c r="D33" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E33" s="400"/>
       <c r="F33" s="400"/>
@@ -34763,7 +34851,7 @@
       <c r="Y33" s="418"/>
       <c r="Z33" s="418"/>
       <c r="AA33" s="407" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="AB33" s="407"/>
       <c r="AC33" s="407"/>
@@ -34771,10 +34859,10 @@
       <c r="AE33" s="407"/>
       <c r="AF33" s="408"/>
       <c r="AG33" s="425" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AH33" s="426" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AI33" s="411"/>
       <c r="AJ33" s="412"/>
@@ -34799,7 +34887,7 @@
         <v>127</v>
       </c>
       <c r="D34" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E34" s="400"/>
       <c r="F34" s="400"/>
@@ -34807,16 +34895,16 @@
       <c r="H34" s="400"/>
       <c r="I34" s="400"/>
       <c r="J34" s="422" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="K34" s="422"/>
       <c r="L34" s="422"/>
       <c r="M34" s="422"/>
       <c r="N34" s="427" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="O34" s="428" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P34" s="32"/>
       <c r="Q34" s="429"/>
@@ -34860,7 +34948,7 @@
         <v>127</v>
       </c>
       <c r="D35" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E35" s="400"/>
       <c r="F35" s="400"/>
@@ -34887,16 +34975,16 @@
       <c r="AA35" s="434"/>
       <c r="AB35" s="434"/>
       <c r="AC35" s="407" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AD35" s="407"/>
       <c r="AE35" s="407"/>
       <c r="AF35" s="435"/>
       <c r="AG35" s="436" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AH35" s="437" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AI35" s="438"/>
       <c r="AJ35" s="439"/>
@@ -34921,7 +35009,7 @@
         <v>127</v>
       </c>
       <c r="D36" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E36" s="400"/>
       <c r="F36" s="400"/>
@@ -34951,7 +35039,7 @@
       <c r="AB36" s="434"/>
       <c r="AC36" s="434"/>
       <c r="AD36" s="407" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="AE36" s="407"/>
       <c r="AF36" s="435"/>
@@ -34984,7 +35072,7 @@
         <v>127</v>
       </c>
       <c r="D37" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E37" s="400"/>
       <c r="F37" s="400"/>
@@ -35015,7 +35103,7 @@
       <c r="AC37" s="434"/>
       <c r="AD37" s="434"/>
       <c r="AE37" s="407" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="AF37" s="435"/>
       <c r="AG37" s="436"/>
@@ -35025,7 +35113,7 @@
         <v>234</v>
       </c>
       <c r="AK37" s="271" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="AL37" s="413"/>
       <c r="AM37" s="440"/>
@@ -35047,7 +35135,7 @@
         <v>127</v>
       </c>
       <c r="D38" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E38" s="400"/>
       <c r="F38" s="400"/>
@@ -35075,15 +35163,15 @@
       <c r="AB38" s="434"/>
       <c r="AC38" s="434"/>
       <c r="AD38" s="407" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="AE38" s="407"/>
       <c r="AF38" s="435"/>
       <c r="AG38" s="425" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AH38" s="426" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AI38" s="438"/>
       <c r="AJ38" s="439"/>
@@ -35108,7 +35196,7 @@
         <v>127</v>
       </c>
       <c r="D39" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E39" s="400"/>
       <c r="F39" s="400"/>
@@ -35119,18 +35207,18 @@
       <c r="K39" s="443"/>
       <c r="L39" s="443"/>
       <c r="M39" s="446" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="N39" s="447"/>
       <c r="O39" s="448"/>
       <c r="P39" s="420" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="Q39" s="421" t="s">
         <v>190</v>
       </c>
       <c r="R39" s="420" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="S39" s="430"/>
       <c r="T39" s="431"/>
@@ -35171,11 +35259,11 @@
         <v>127</v>
       </c>
       <c r="D40" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E40" s="400"/>
       <c r="F40" s="422" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="G40" s="422"/>
       <c r="H40" s="422"/>
@@ -35185,19 +35273,19 @@
       <c r="L40" s="422"/>
       <c r="M40" s="422"/>
       <c r="N40" s="401" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="O40" s="402" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P40" s="403"/>
       <c r="Q40" s="404"/>
       <c r="R40" s="403"/>
       <c r="S40" s="401" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="T40" s="402" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="U40" s="405"/>
       <c r="V40" s="406"/>
@@ -35236,12 +35324,12 @@
         <v>127</v>
       </c>
       <c r="D41" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E41" s="400"/>
       <c r="F41" s="422"/>
       <c r="G41" s="422" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="H41" s="422"/>
       <c r="I41" s="422"/>
@@ -35257,7 +35345,7 @@
       <c r="S41" s="401"/>
       <c r="T41" s="402"/>
       <c r="U41" s="424" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="V41" s="406"/>
       <c r="W41" s="418"/>
@@ -35295,7 +35383,7 @@
         <v>127</v>
       </c>
       <c r="D42" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E42" s="400"/>
       <c r="F42" s="400"/>
@@ -35318,7 +35406,7 @@
       <c r="W42" s="418"/>
       <c r="X42" s="418"/>
       <c r="Y42" s="407" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="Z42" s="407"/>
       <c r="AA42" s="407"/>
@@ -35328,10 +35416,10 @@
       <c r="AE42" s="407"/>
       <c r="AF42" s="408"/>
       <c r="AG42" s="409" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AH42" s="410" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AI42" s="411"/>
       <c r="AJ42" s="412"/>
@@ -35356,7 +35444,7 @@
         <v>127</v>
       </c>
       <c r="D43" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E43" s="400"/>
       <c r="F43" s="400"/>
@@ -35382,7 +35470,7 @@
       <c r="X43" s="418"/>
       <c r="Y43" s="418"/>
       <c r="Z43" s="407" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="AA43" s="407"/>
       <c r="AB43" s="407"/>
@@ -35419,7 +35507,7 @@
         <v>127</v>
       </c>
       <c r="D44" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E44" s="400"/>
       <c r="F44" s="400"/>
@@ -35444,7 +35532,7 @@
       <c r="Y44" s="418"/>
       <c r="Z44" s="418"/>
       <c r="AA44" s="407" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="AB44" s="407"/>
       <c r="AC44" s="407"/>
@@ -35476,7 +35564,7 @@
         <v>127</v>
       </c>
       <c r="D45" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E45" s="400"/>
       <c r="F45" s="400"/>
@@ -35500,7 +35588,7 @@
       <c r="X45" s="418"/>
       <c r="Y45" s="418"/>
       <c r="Z45" s="407" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="AA45" s="407"/>
       <c r="AB45" s="407"/>
@@ -35537,7 +35625,7 @@
         <v>127</v>
       </c>
       <c r="D46" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E46" s="400"/>
       <c r="F46" s="400"/>
@@ -35564,7 +35652,7 @@
       <c r="Y46" s="418"/>
       <c r="Z46" s="418"/>
       <c r="AA46" s="407" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="AB46" s="407"/>
       <c r="AC46" s="407"/>
@@ -35600,7 +35688,7 @@
         <v>127</v>
       </c>
       <c r="D47" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E47" s="400"/>
       <c r="F47" s="400"/>
@@ -35628,7 +35716,7 @@
       <c r="Z47" s="418"/>
       <c r="AA47" s="418"/>
       <c r="AB47" s="407" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="AC47" s="407"/>
       <c r="AD47" s="407"/>
@@ -35641,7 +35729,7 @@
         <v>234</v>
       </c>
       <c r="AK47" s="210" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="AL47" s="413"/>
       <c r="AM47" s="414"/>
@@ -35663,7 +35751,7 @@
         <v>127</v>
       </c>
       <c r="D48" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E48" s="400"/>
       <c r="F48" s="400"/>
@@ -35688,7 +35776,7 @@
       <c r="Y48" s="418"/>
       <c r="Z48" s="418"/>
       <c r="AA48" s="407" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="AB48" s="407"/>
       <c r="AC48" s="407"/>
@@ -35696,10 +35784,10 @@
       <c r="AE48" s="407"/>
       <c r="AF48" s="408"/>
       <c r="AG48" s="425" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AH48" s="426" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AI48" s="411"/>
       <c r="AJ48" s="412"/>
@@ -35724,7 +35812,7 @@
         <v>127</v>
       </c>
       <c r="D49" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E49" s="400"/>
       <c r="F49" s="400"/>
@@ -35738,10 +35826,10 @@
       <c r="L49" s="422"/>
       <c r="M49" s="422"/>
       <c r="N49" s="427" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="O49" s="449" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P49" s="32"/>
       <c r="Q49" s="429"/>
@@ -35785,7 +35873,7 @@
         <v>127</v>
       </c>
       <c r="D50" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E50" s="400"/>
       <c r="F50" s="400"/>
@@ -35812,16 +35900,16 @@
       <c r="AA50" s="434"/>
       <c r="AB50" s="434"/>
       <c r="AC50" s="407" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="AD50" s="407"/>
       <c r="AE50" s="407"/>
       <c r="AF50" s="435"/>
       <c r="AG50" s="436" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AH50" s="437" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AI50" s="438"/>
       <c r="AJ50" s="439"/>
@@ -35846,7 +35934,7 @@
         <v>127</v>
       </c>
       <c r="D51" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E51" s="400"/>
       <c r="F51" s="400"/>
@@ -35876,7 +35964,7 @@
       <c r="AB51" s="434"/>
       <c r="AC51" s="434"/>
       <c r="AD51" s="407" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="AE51" s="407"/>
       <c r="AF51" s="435"/>
@@ -35909,7 +35997,7 @@
         <v>127</v>
       </c>
       <c r="D52" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E52" s="400"/>
       <c r="F52" s="400"/>
@@ -35940,7 +36028,7 @@
       <c r="AC52" s="434"/>
       <c r="AD52" s="434"/>
       <c r="AE52" s="407" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AF52" s="435"/>
       <c r="AG52" s="436"/>
@@ -35950,7 +36038,7 @@
         <v>234</v>
       </c>
       <c r="AK52" s="271" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="AL52" s="413"/>
       <c r="AM52" s="440"/>
@@ -35972,7 +36060,7 @@
         <v>127</v>
       </c>
       <c r="D53" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E53" s="400"/>
       <c r="F53" s="400"/>
@@ -36000,15 +36088,15 @@
       <c r="AB53" s="434"/>
       <c r="AC53" s="434"/>
       <c r="AD53" s="407" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="AE53" s="407"/>
       <c r="AF53" s="435"/>
       <c r="AG53" s="425" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AH53" s="426" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AI53" s="438"/>
       <c r="AJ53" s="439"/>
@@ -36033,7 +36121,7 @@
         <v>127</v>
       </c>
       <c r="D54" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E54" s="400"/>
       <c r="F54" s="400"/>
@@ -36044,18 +36132,18 @@
       <c r="K54" s="443"/>
       <c r="L54" s="443"/>
       <c r="M54" s="446" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="N54" s="447"/>
       <c r="O54" s="448"/>
       <c r="P54" s="420" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="Q54" s="421" t="s">
         <v>190</v>
       </c>
       <c r="R54" s="420" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="S54" s="430"/>
       <c r="T54" s="431"/>
@@ -36096,7 +36184,7 @@
         <v>127</v>
       </c>
       <c r="D55" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E55" s="400"/>
       <c r="F55" s="400"/>
@@ -36115,10 +36203,10 @@
       <c r="Q55" s="429"/>
       <c r="R55" s="32"/>
       <c r="S55" s="430" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="T55" s="431" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="U55" s="432"/>
       <c r="V55" s="433"/>
@@ -36301,12 +36389,12 @@
   </sheetPr>
   <dimension ref="A1:AW10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="13" ySplit="4" topLeftCell="N5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="U9" activeCellId="0" sqref="U9"/>
+      <selection pane="bottomRight" activeCell="U8" activeCellId="0" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36352,7 +36440,7 @@
       </c>
       <c r="D1" s="372"/>
       <c r="E1" s="373" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F1" s="373"/>
       <c r="G1" s="373"/>
@@ -36363,7 +36451,7 @@
       <c r="L1" s="373"/>
       <c r="M1" s="373"/>
       <c r="N1" s="373" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="O1" s="373"/>
       <c r="P1" s="373"/>
@@ -36372,7 +36460,7 @@
       <c r="S1" s="373"/>
       <c r="T1" s="373"/>
       <c r="U1" s="374" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="V1" s="375" t="s">
         <v>111</v>
@@ -36399,7 +36487,7 @@
       <c r="AN1" s="276"/>
       <c r="AO1" s="276"/>
       <c r="AP1" s="376" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AQ1" s="376"/>
       <c r="AR1" s="376"/>
@@ -36423,7 +36511,7 @@
         <v>116</v>
       </c>
       <c r="E2" s="380" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F2" s="380"/>
       <c r="G2" s="380"/>
@@ -36434,20 +36522,20 @@
       <c r="L2" s="380"/>
       <c r="M2" s="380"/>
       <c r="N2" s="380" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="O2" s="380"/>
       <c r="P2" s="373" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="Q2" s="373"/>
       <c r="R2" s="373"/>
       <c r="S2" s="380" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="T2" s="380"/>
       <c r="U2" s="376" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="V2" s="375" t="s">
         <v>117</v>
@@ -36505,7 +36593,7 @@
       <c r="L3" s="373"/>
       <c r="M3" s="373"/>
       <c r="N3" s="382" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="O3" s="382"/>
       <c r="P3" s="373" t="s">
@@ -36515,10 +36603,10 @@
         <v>121</v>
       </c>
       <c r="R3" s="373" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="S3" s="382" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="T3" s="382"/>
       <c r="U3" s="374" t="s">
@@ -36658,7 +36746,7 @@
         <v>38</v>
       </c>
       <c r="B5" s="389" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C5" s="390"/>
       <c r="D5" s="390"/>
@@ -36715,7 +36803,7 @@
         <v>127</v>
       </c>
       <c r="D6" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E6" s="400"/>
       <c r="F6" s="400"/>
@@ -36736,7 +36824,7 @@
       <c r="U6" s="405"/>
       <c r="V6" s="406"/>
       <c r="W6" s="407" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="X6" s="407"/>
       <c r="Y6" s="407"/>
@@ -36748,10 +36836,10 @@
       <c r="AE6" s="407"/>
       <c r="AF6" s="408"/>
       <c r="AG6" s="409" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AH6" s="410" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AI6" s="411"/>
       <c r="AJ6" s="412"/>
@@ -36776,7 +36864,7 @@
         <v>127</v>
       </c>
       <c r="D7" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E7" s="400"/>
       <c r="F7" s="400"/>
@@ -36817,7 +36905,7 @@
       <c r="AI7" s="411"/>
       <c r="AJ7" s="412"/>
       <c r="AK7" s="210" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AL7" s="413"/>
       <c r="AM7" s="414"/>
@@ -36839,10 +36927,10 @@
         <v>127</v>
       </c>
       <c r="D8" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E8" s="400" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="F8" s="400"/>
       <c r="G8" s="400"/>
@@ -36853,19 +36941,19 @@
       <c r="L8" s="400"/>
       <c r="M8" s="400"/>
       <c r="N8" s="401" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="O8" s="402" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P8" s="403"/>
       <c r="Q8" s="404"/>
       <c r="R8" s="403"/>
       <c r="S8" s="401" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="T8" s="402" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="U8" s="405"/>
       <c r="V8" s="406"/>
@@ -36904,11 +36992,11 @@
         <v>127</v>
       </c>
       <c r="D9" s="399" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E9" s="400"/>
       <c r="F9" s="400" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="G9" s="400"/>
       <c r="H9" s="400"/>
@@ -36924,8 +37012,8 @@
       <c r="R9" s="403"/>
       <c r="S9" s="401"/>
       <c r="T9" s="402"/>
-      <c r="U9" s="405" t="s">
-        <v>527</v>
+      <c r="U9" s="421" t="s">
+        <v>528</v>
       </c>
       <c r="V9" s="406"/>
       <c r="W9" s="407"/>
@@ -37310,7 +37398,7 @@
         <v>37</v>
       </c>
       <c r="B5" s="74" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C5" s="75"/>
       <c r="D5" s="75"/>
@@ -37345,11 +37433,11 @@
         <v>127</v>
       </c>
       <c r="D6" s="81" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E6" s="460"/>
       <c r="F6" s="461" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="G6" s="461"/>
       <c r="H6" s="461"/>
@@ -37384,12 +37472,12 @@
         <v>127</v>
       </c>
       <c r="D7" s="81" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E7" s="467"/>
       <c r="F7" s="468"/>
       <c r="G7" s="468" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="H7" s="468"/>
       <c r="I7" s="468"/>
@@ -37405,13 +37493,13 @@
       <c r="Q7" s="472"/>
       <c r="R7" s="467"/>
       <c r="S7" s="473" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="T7" s="469"/>
       <c r="U7" s="470"/>
       <c r="V7" s="471"/>
       <c r="W7" s="469" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="X7" s="68"/>
       <c r="Y7" s="57"/>
@@ -37425,12 +37513,12 @@
         <v>127</v>
       </c>
       <c r="D8" s="81" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E8" s="467"/>
       <c r="F8" s="468"/>
       <c r="G8" s="468" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="H8" s="468"/>
       <c r="I8" s="468"/>
@@ -37446,13 +37534,13 @@
       <c r="Q8" s="472"/>
       <c r="R8" s="467"/>
       <c r="S8" s="473" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="T8" s="469"/>
       <c r="U8" s="470"/>
       <c r="V8" s="471"/>
       <c r="W8" s="469" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="X8" s="68"/>
       <c r="Y8" s="57"/>
@@ -37466,12 +37554,12 @@
         <v>127</v>
       </c>
       <c r="D9" s="81" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E9" s="467"/>
       <c r="F9" s="468"/>
       <c r="G9" s="468" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="H9" s="468"/>
       <c r="I9" s="468"/>
@@ -37487,13 +37575,13 @@
       <c r="Q9" s="472"/>
       <c r="R9" s="467"/>
       <c r="S9" s="473" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="T9" s="469"/>
       <c r="U9" s="470"/>
       <c r="V9" s="471"/>
       <c r="W9" s="469" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="X9" s="68"/>
       <c r="Y9" s="57"/>
@@ -37507,12 +37595,12 @@
         <v>127</v>
       </c>
       <c r="D10" s="81" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E10" s="467"/>
       <c r="F10" s="468"/>
       <c r="G10" s="468" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="H10" s="468"/>
       <c r="I10" s="468"/>
@@ -37528,13 +37616,13 @@
       <c r="Q10" s="472"/>
       <c r="R10" s="467"/>
       <c r="S10" s="473" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="T10" s="469"/>
       <c r="U10" s="470"/>
       <c r="V10" s="471"/>
       <c r="W10" s="469" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="X10" s="68"/>
       <c r="Y10" s="57"/>

</xml_diff>